<commit_message>
updated order - april 6
</commit_message>
<xml_diff>
--- a/nfl_draft_order_2022.xlsx
+++ b/nfl_draft_order_2022.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UALR\Artificial Intelligence\borromeoz-mock-draft\NFL-Mock-Draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02F697B-3EEB-442F-A979-75F3767F3745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4419C4-F302-483B-955D-C9F2F24D0C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0EE48182-35F7-435F-BF15-1CF975F50B78}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="11295" xr2:uid="{0EE48182-35F7-435F-BF15-1CF975F50B78}"/>
   </bookViews>
   <sheets>
-    <sheet name="last updated - march 23" sheetId="1" r:id="rId1"/>
+    <sheet name="last updated - april 6" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -519,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE60D276-7719-494F-8337-51BCCB53B1E0}">
   <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D94" sqref="D1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,7 +737,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>